<commit_message>
final calculations of emissions, time, money saved
</commit_message>
<xml_diff>
--- a/data/calculations.xlsx
+++ b/data/calculations.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizziehealy/Desktop/DSAN_5550/Final Project/Greener_Pastures/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1E056D-0212-374E-BD18-14F8BCF1F112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB01FF07-296D-144E-AC87-2466F808579E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="5340" windowWidth="27980" windowHeight="16920" xr2:uid="{EE571B13-C74D-AB42-ABB6-12E148D49AF2}"/>
+    <workbookView xWindow="760" yWindow="800" windowWidth="27980" windowHeight="16920" xr2:uid="{EE571B13-C74D-AB42-ABB6-12E148D49AF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="130">
   <si>
     <t>vehicle</t>
   </si>
@@ -411,13 +411,28 @@
   </si>
   <si>
     <t>Tot Distance</t>
+  </si>
+  <si>
+    <t>w/ MF</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>w/o MF</t>
+  </si>
+  <si>
+    <t>*w/ MF means I include driving from Media Florist at beginning of delivery trip</t>
+  </si>
+  <si>
+    <t>and returning to Media Florist at end of trip</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -427,6 +442,12 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -501,7 +522,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -509,11 +530,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -526,6 +576,23 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -860,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F6CAC6-FC57-AC47-808A-3F4B655536A1}">
-  <dimension ref="A1:L103"/>
+  <dimension ref="A1:N113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N100" sqref="N100"/>
+    <sheetView tabSelected="1" topLeftCell="C84" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O107" sqref="O107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -871,7 +938,7 @@
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -902,11 +969,14 @@
       <c r="K1" t="s">
         <v>123</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="12" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -928,8 +998,15 @@
       <c r="G2" s="1">
         <v>-75.373343052110002</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L2" s="12"/>
+      <c r="M2">
+        <v>6</v>
+      </c>
+      <c r="N2">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -957,8 +1034,9 @@
       <c r="I3" s="1">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L3" s="12"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -986,8 +1064,9 @@
       <c r="I4" s="1">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L4" s="12"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1015,8 +1094,9 @@
       <c r="I5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L5" s="12"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -1044,8 +1124,9 @@
       <c r="I6" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L6" s="12"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1073,8 +1154,9 @@
       <c r="I7" s="1">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L7" s="12"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1102,8 +1184,9 @@
       <c r="I8" s="1">
         <v>13.8</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L8" s="12"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1131,8 +1214,9 @@
       <c r="I9" s="1">
         <v>7.8</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L9" s="12"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1160,8 +1244,15 @@
       <c r="I10" s="1">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L10" s="12"/>
+      <c r="M10">
+        <v>5</v>
+      </c>
+      <c r="N10">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1193,12 +1284,12 @@
         <f>SUM(H3:H11)</f>
         <v>117</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="13">
         <f>SUM(I3:I11)</f>
         <v>42.1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>2</v>
       </c>
@@ -1220,8 +1311,15 @@
       <c r="G12" s="2">
         <v>-75.45482624412</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L12" s="12"/>
+      <c r="M12">
+        <v>10</v>
+      </c>
+      <c r="N12">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>2</v>
       </c>
@@ -1249,8 +1347,9 @@
       <c r="I13" s="2">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L13" s="12"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>2</v>
       </c>
@@ -1278,8 +1377,9 @@
       <c r="I14" s="2">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L14" s="12"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>2</v>
       </c>
@@ -1307,8 +1407,9 @@
       <c r="I15" s="2">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L15" s="12"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>2</v>
       </c>
@@ -1336,8 +1437,9 @@
       <c r="I16" s="2">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L16" s="12"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>2</v>
       </c>
@@ -1365,8 +1467,9 @@
       <c r="I17" s="2">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L17" s="12"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>2</v>
       </c>
@@ -1394,8 +1497,9 @@
       <c r="I18" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L18" s="12"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>2</v>
       </c>
@@ -1423,8 +1527,9 @@
       <c r="I19" s="2">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L19" s="12"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>2</v>
       </c>
@@ -1452,8 +1557,15 @@
       <c r="I20" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L20" s="12"/>
+      <c r="M20">
+        <v>8</v>
+      </c>
+      <c r="N20">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>2</v>
       </c>
@@ -1485,12 +1597,12 @@
         <f>SUM(H13:H21)</f>
         <v>46</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L21" s="14">
         <f>SUM(I13:I21)</f>
         <v>19.3</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>3</v>
       </c>
@@ -1512,8 +1624,15 @@
       <c r="G22" s="3">
         <v>-75.350921378039004</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L22" s="12"/>
+      <c r="M22">
+        <v>8</v>
+      </c>
+      <c r="N22">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>3</v>
       </c>
@@ -1541,8 +1660,9 @@
       <c r="I23" s="3">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L23" s="12"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>3</v>
       </c>
@@ -1570,8 +1690,9 @@
       <c r="I24" s="3">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L24" s="12"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>3</v>
       </c>
@@ -1599,8 +1720,9 @@
       <c r="I25" s="3">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L25" s="12"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>3</v>
       </c>
@@ -1628,8 +1750,9 @@
       <c r="I26" s="3">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L26" s="12"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>3</v>
       </c>
@@ -1657,8 +1780,9 @@
       <c r="I27" s="3">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L27" s="12"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>3</v>
       </c>
@@ -1686,8 +1810,9 @@
       <c r="I28" s="3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L28" s="12"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>3</v>
       </c>
@@ -1715,8 +1840,9 @@
       <c r="I29" s="3">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L29" s="12"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>3</v>
       </c>
@@ -1744,8 +1870,15 @@
       <c r="I30" s="3">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L30" s="12"/>
+      <c r="M30">
+        <v>10</v>
+      </c>
+      <c r="N30">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>3</v>
       </c>
@@ -1777,12 +1910,12 @@
         <f>SUM(H23:H31)</f>
         <v>52</v>
       </c>
-      <c r="L31" s="3">
+      <c r="L31" s="15">
         <f>SUM(I23:I31)</f>
         <v>12.899999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>4</v>
       </c>
@@ -1804,8 +1937,15 @@
       <c r="G32" s="4">
         <v>-75.419262725086</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L32" s="12"/>
+      <c r="M32">
+        <v>9</v>
+      </c>
+      <c r="N32">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>4</v>
       </c>
@@ -1833,8 +1973,9 @@
       <c r="I33" s="4">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L33" s="12"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>4</v>
       </c>
@@ -1862,8 +2003,9 @@
       <c r="I34" s="4">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L34" s="12"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>4</v>
       </c>
@@ -1891,8 +2033,9 @@
       <c r="I35" s="4">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L35" s="12"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>4</v>
       </c>
@@ -1920,8 +2063,9 @@
       <c r="I36" s="4">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L36" s="12"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>4</v>
       </c>
@@ -1949,8 +2093,9 @@
       <c r="I37" s="4">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L37" s="12"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>4</v>
       </c>
@@ -1978,8 +2123,9 @@
       <c r="I38" s="4">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L38" s="12"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>4</v>
       </c>
@@ -2007,8 +2153,9 @@
       <c r="I39" s="4">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L39" s="12"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>4</v>
       </c>
@@ -2036,8 +2183,15 @@
       <c r="I40" s="4">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L40" s="12"/>
+      <c r="M40">
+        <v>11</v>
+      </c>
+      <c r="N40">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>4</v>
       </c>
@@ -2069,12 +2223,12 @@
         <f>SUM(H33:H41)</f>
         <v>28</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L41" s="16">
         <f>SUM(I33:I41)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
         <v>5</v>
       </c>
@@ -2096,8 +2250,15 @@
       <c r="G42" s="5">
         <v>-75.375889718498001</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L42" s="12"/>
+      <c r="M42">
+        <v>5</v>
+      </c>
+      <c r="N42">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
         <v>5</v>
       </c>
@@ -2125,8 +2286,9 @@
       <c r="I43" s="5">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L43" s="12"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>5</v>
       </c>
@@ -2154,8 +2316,9 @@
       <c r="I44" s="5">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L44" s="12"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>5</v>
       </c>
@@ -2183,8 +2346,9 @@
       <c r="I45" s="5">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L45" s="12"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
         <v>5</v>
       </c>
@@ -2212,8 +2376,9 @@
       <c r="I46" s="5">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L46" s="12"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>5</v>
       </c>
@@ -2241,8 +2406,9 @@
       <c r="I47" s="5">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L47" s="12"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
         <v>5</v>
       </c>
@@ -2270,8 +2436,9 @@
       <c r="I48" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L48" s="12"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
         <v>5</v>
       </c>
@@ -2299,8 +2466,9 @@
       <c r="I49" s="5">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L49" s="12"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
         <v>5</v>
       </c>
@@ -2328,8 +2496,15 @@
       <c r="I50" s="5">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L50" s="12"/>
+      <c r="M50">
+        <v>5</v>
+      </c>
+      <c r="N50">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
         <v>5</v>
       </c>
@@ -2361,12 +2536,12 @@
         <f>SUM(H43:H51)</f>
         <v>23</v>
       </c>
-      <c r="L51" s="5">
+      <c r="L51" s="17">
         <f>SUM(I43:I51)</f>
         <v>6.1000000000000005</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>6</v>
       </c>
@@ -2388,8 +2563,15 @@
       <c r="G52" s="6">
         <v>-75.392068185967005</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L52" s="12"/>
+      <c r="M52">
+        <v>4</v>
+      </c>
+      <c r="N52">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>6</v>
       </c>
@@ -2417,8 +2599,9 @@
       <c r="I53" s="6">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L53" s="12"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>6</v>
       </c>
@@ -2446,8 +2629,9 @@
       <c r="I54" s="6">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L54" s="12"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="6">
         <v>6</v>
       </c>
@@ -2475,8 +2659,9 @@
       <c r="I55" s="6">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L55" s="12"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
         <v>6</v>
       </c>
@@ -2504,8 +2689,9 @@
       <c r="I56" s="6">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L56" s="12"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
         <v>6</v>
       </c>
@@ -2533,8 +2719,9 @@
       <c r="I57" s="6">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L57" s="12"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
         <v>6</v>
       </c>
@@ -2562,8 +2749,9 @@
       <c r="I58" s="6">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L58" s="12"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
         <v>6</v>
       </c>
@@ -2591,8 +2779,9 @@
       <c r="I59" s="6">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L59" s="12"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
         <v>6</v>
       </c>
@@ -2620,8 +2809,15 @@
       <c r="I60" s="6">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L60" s="12"/>
+      <c r="M60">
+        <v>2</v>
+      </c>
+      <c r="N60">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
         <v>6</v>
       </c>
@@ -2653,12 +2849,12 @@
         <f>SUM(H53:H61)</f>
         <v>25</v>
       </c>
-      <c r="L61" s="6">
+      <c r="L61" s="18">
         <f>SUM(I53:I61)</f>
         <v>7.3999999999999995</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
         <v>7</v>
       </c>
@@ -2680,8 +2876,15 @@
       <c r="G62" s="7">
         <v>-75.38232061363</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L62" s="12"/>
+      <c r="M62">
+        <v>5</v>
+      </c>
+      <c r="N62">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
         <v>7</v>
       </c>
@@ -2709,8 +2912,9 @@
       <c r="I63" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L63" s="12"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="7">
         <v>7</v>
       </c>
@@ -2738,8 +2942,9 @@
       <c r="I64" s="7">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L64" s="12"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
         <v>7</v>
       </c>
@@ -2767,8 +2972,9 @@
       <c r="I65" s="7">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L65" s="12"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
         <v>7</v>
       </c>
@@ -2796,8 +3002,9 @@
       <c r="I66" s="7">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L66" s="12"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
         <v>7</v>
       </c>
@@ -2825,8 +3032,9 @@
       <c r="I67" s="7">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L67" s="12"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
         <v>7</v>
       </c>
@@ -2854,8 +3062,9 @@
       <c r="I68" s="7">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L68" s="12"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
         <v>7</v>
       </c>
@@ -2883,8 +3092,9 @@
       <c r="I69" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L69" s="12"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
         <v>7</v>
       </c>
@@ -2912,8 +3122,15 @@
       <c r="I70" s="7">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L70" s="12"/>
+      <c r="M70">
+        <v>5</v>
+      </c>
+      <c r="N70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
         <v>7</v>
       </c>
@@ -2945,12 +3162,12 @@
         <f>SUM(H63:H71)</f>
         <v>24</v>
       </c>
-      <c r="L71" s="7">
+      <c r="L71" s="19">
         <f>SUM(I63:I71)</f>
         <v>6.9</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="8">
         <v>8</v>
       </c>
@@ -2972,8 +3189,15 @@
       <c r="G72" s="8">
         <v>-75.389449262324007</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L72" s="12"/>
+      <c r="M72">
+        <v>3</v>
+      </c>
+      <c r="N72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="8">
         <v>8</v>
       </c>
@@ -3001,8 +3225,9 @@
       <c r="I73" s="8">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L73" s="12"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="8">
         <v>8</v>
       </c>
@@ -3030,8 +3255,9 @@
       <c r="I74" s="8">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L74" s="12"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="8">
         <v>8</v>
       </c>
@@ -3059,8 +3285,9 @@
       <c r="I75" s="8">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L75" s="12"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="8">
         <v>8</v>
       </c>
@@ -3088,8 +3315,9 @@
       <c r="I76" s="8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L76" s="12"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="8">
         <v>8</v>
       </c>
@@ -3117,8 +3345,9 @@
       <c r="I77" s="8">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L77" s="12"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="8">
         <v>8</v>
       </c>
@@ -3146,8 +3375,9 @@
       <c r="I78" s="8">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L78" s="12"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="8">
         <v>8</v>
       </c>
@@ -3175,8 +3405,9 @@
       <c r="I79" s="8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L79" s="12"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="8">
         <v>8</v>
       </c>
@@ -3204,8 +3435,15 @@
       <c r="I80" s="8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L80" s="12"/>
+      <c r="M80">
+        <v>6</v>
+      </c>
+      <c r="N80">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="8">
         <v>8</v>
       </c>
@@ -3237,12 +3475,12 @@
         <f>SUM(H73:H81)</f>
         <v>18</v>
       </c>
-      <c r="L81" s="8">
+      <c r="L81" s="20">
         <f>SUM(I73:I81)</f>
         <v>6.1</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="9">
         <v>9</v>
       </c>
@@ -3264,8 +3502,15 @@
       <c r="G82" s="9">
         <v>-75.377465643733004</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L82" s="12"/>
+      <c r="M82">
+        <v>2</v>
+      </c>
+      <c r="N82">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="9">
         <v>9</v>
       </c>
@@ -3293,8 +3538,9 @@
       <c r="I83" s="9">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L83" s="12"/>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="9">
         <v>9</v>
       </c>
@@ -3322,8 +3568,9 @@
       <c r="I84" s="9">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L84" s="12"/>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="9">
         <v>9</v>
       </c>
@@ -3351,8 +3598,9 @@
       <c r="I85" s="9">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L85" s="12"/>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="9">
         <v>9</v>
       </c>
@@ -3380,8 +3628,9 @@
       <c r="I86" s="9">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L86" s="12"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="9">
         <v>9</v>
       </c>
@@ -3409,8 +3658,9 @@
       <c r="I87" s="9">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L87" s="12"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="9">
         <v>9</v>
       </c>
@@ -3438,8 +3688,9 @@
       <c r="I88" s="9">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L88" s="12"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="9">
         <v>9</v>
       </c>
@@ -3467,8 +3718,15 @@
       <c r="I89" s="9">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L89" s="12"/>
+      <c r="M89">
+        <v>3</v>
+      </c>
+      <c r="N89">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="9">
         <v>9</v>
       </c>
@@ -3500,12 +3758,12 @@
         <f>SUM(H83:H90)</f>
         <v>22</v>
       </c>
-      <c r="L90" s="9">
+      <c r="L90" s="21">
         <f>SUM(I83:I90)</f>
         <v>6.8</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="10">
         <v>10</v>
       </c>
@@ -3527,8 +3785,15 @@
       <c r="G91" s="10">
         <v>-75.381501317347997</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L91" s="12"/>
+      <c r="M91">
+        <v>4</v>
+      </c>
+      <c r="N91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="10">
         <v>10</v>
       </c>
@@ -3556,8 +3821,9 @@
       <c r="I92" s="10">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L92" s="12"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="10">
         <v>10</v>
       </c>
@@ -3585,8 +3851,9 @@
       <c r="I93" s="10">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L93" s="12"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="10">
         <v>10</v>
       </c>
@@ -3614,8 +3881,9 @@
       <c r="I94" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L94" s="12"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="10">
         <v>10</v>
       </c>
@@ -3643,8 +3911,9 @@
       <c r="I95" s="10">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L95" s="12"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="10">
         <v>10</v>
       </c>
@@ -3672,8 +3941,9 @@
       <c r="I96" s="10">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L96" s="12"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="10">
         <v>10</v>
       </c>
@@ -3701,8 +3971,9 @@
       <c r="I97" s="10">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L97" s="12"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="10">
         <v>10</v>
       </c>
@@ -3730,8 +4001,9 @@
       <c r="I98" s="10">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L98" s="12"/>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" s="10">
         <v>10</v>
       </c>
@@ -3759,8 +4031,15 @@
       <c r="I99" s="10">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L99" s="12"/>
+      <c r="M99">
+        <v>4</v>
+      </c>
+      <c r="N99">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="10">
         <v>10</v>
       </c>
@@ -3792,25 +4071,86 @@
         <f>SUM(H92:H100)</f>
         <v>24</v>
       </c>
-      <c r="L100" s="10">
+      <c r="L100" s="22">
         <f>SUM(I92:I100)</f>
         <v>5.8999999999999995</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K102" s="11">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L101" s="12"/>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K102" s="27">
         <f>K11+K21+K31+K41+K51+K61+K71+K81+K90+K100</f>
         <v>379</v>
       </c>
-      <c r="L102" s="11">
+      <c r="L102" s="28">
         <f>L11+L21+L31+L41+L51+L61+L71+L81+L90+L100</f>
         <v>122.50000000000001</v>
       </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M102">
+        <f>SUM(M2:M99)</f>
+        <v>115</v>
+      </c>
+      <c r="N102">
+        <f>SUM(N2:N99)</f>
+        <v>40.900000000000006</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="K103">
         <f>K102/60</f>
         <v>6.3166666666666664</v>
+      </c>
+      <c r="L103" s="12"/>
+      <c r="M103">
+        <f>K102+M102</f>
+        <v>494</v>
+      </c>
+      <c r="N103">
+        <f>L102+N102</f>
+        <v>163.40000000000003</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K107" s="25"/>
+      <c r="L107" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="M107" s="26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K108" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="L108" s="11">
+        <v>379</v>
+      </c>
+      <c r="M108" s="11">
+        <v>122.5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K109" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="L109" s="11">
+        <v>494</v>
+      </c>
+      <c r="M109" s="11">
+        <v>163.4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K112" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="113" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K113" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>